<commit_message>
added models with 100 epochs, 32 batch for all datasets
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo ThinkBook\Documents\Thesis\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF1FD4E-29D8-4F99-92A5-5E7688FA6603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349B7196-E31A-47B7-888D-10B626D21902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="25">
   <si>
     <t>Epochs</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>2.008 hours</t>
+  </si>
+  <si>
+    <t>512x512</t>
+  </si>
+  <si>
+    <t>320x320</t>
+  </si>
+  <si>
+    <t>Training</t>
   </si>
 </sst>
 </file>
@@ -162,7 +171,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -449,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -464,7 +480,7 @@
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -585,7 +601,7 @@
         <v>7</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I13" si="0">_xlfn.CONCAT(C3, "_", D3, "e_",E3, "p_",F3, "b_",G3, "_",A3,"_",B3)</f>
+        <f t="shared" ref="I3:I12" si="0">_xlfn.CONCAT(C3, "_", D3, "e_",E3, "p_",F3, "b_",G3, "_",A3,"_",B3)</f>
         <v>yolov8n_100e_0p_16b_Adam_640x640_0.2</v>
       </c>
     </row>
@@ -876,35 +892,8 @@
         <v>8</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C13, "_", D13, "e_",E13, "p_",F13, "b_",G13, "_",A13,"_",B13)</f>
         <v>yolov8n_300e_50p_32b_SGD_640x640_0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1">
-        <v>100</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>16</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="1" t="str">
-        <f>_xlfn.CONCAT(C14, "_", D14, "e_",E14, "p_",F14, "b_",G14, "_",A14,"_",B14)</f>
-        <v>yolov8n_100e_0p_16b_auto_640x640_0.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -912,7 +901,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -924,14 +913,17 @@
         <v>0</v>
       </c>
       <c r="F15" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f t="shared" ref="I15:I25" si="1">_xlfn.CONCAT(C15, "_", D15, "e_",E15, "p_",F15, "b_",G15, "_",A15,"_",B15)</f>
-        <v>yolov8n_100e_0p_16b_Adam_640x640_0.1</v>
+        <f t="shared" ref="I15:I17" si="1">_xlfn.CONCAT(C15, "_", D15, "e_",E15, "p_",F15, "b_",G15, "_",A15,"_",B15)</f>
+        <v>yolov8n_100e_0p_32b_auto_640x640_0.06</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -939,7 +931,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -951,14 +943,14 @@
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>yolov8n_100e_0p_16b_SGD_640x640_0.1</v>
+        <v>yolov8n_100e_0p_32b_Adam_640x640_0.06</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -966,7 +958,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
@@ -981,11 +973,11 @@
         <v>32</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>yolov8n_100e_0p_32b_auto_640x640_0.1</v>
+        <v>yolov8n_100e_0p_32b_SGD_640x640_0.06</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -993,7 +985,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>6</v>
@@ -1005,14 +997,14 @@
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_100e_0p_32b_Adam_640x640_0.1</v>
+        <f t="shared" ref="I18:I20" si="2">_xlfn.CONCAT(C18, "_", D18, "e_",E18, "p_",F18, "b_",G18, "_",A18,"_",B18)</f>
+        <v>yolov8n_100e_0p_16b_auto_640x640_0.06</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1020,7 +1012,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
@@ -1032,14 +1024,14 @@
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_100e_0p_32b_SGD_640x640_0.1</v>
+        <f t="shared" si="2"/>
+        <v>yolov8n_100e_0p_16b_Adam_640x640_0.06</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1047,170 +1039,541 @@
         <v>14</v>
       </c>
       <c r="B20" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
         <v>16</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_300e_50p_16b_auto_640x640_0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1">
-        <v>300</v>
-      </c>
-      <c r="E21" s="1">
-        <v>50</v>
-      </c>
-      <c r="F21" s="1">
-        <v>16</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_300e_50p_16b_Adam_640x640_0.1</v>
+        <f t="shared" si="2"/>
+        <v>yolov8n_100e_0p_16b_SGD_640x640_0.06</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_300e_50p_16b_SGD_640x640_0.1</v>
+        <f t="shared" ref="I22:I27" si="3">_xlfn.CONCAT(C22, "_", D22, "e_",E22, "p_",F22, "b_",G22, "_",A22,"_",B22)</f>
+        <v>yolov8n_100e_0p_32b_auto_512x512_0.07</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1">
         <v>32</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_300e_50p_32b_auto_640x640_0.1</v>
+        <f t="shared" si="3"/>
+        <v>yolov8n_100e_0p_32b_Adam_512x512_0.07</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
         <v>32</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_300e_50p_32b_Adam_640x640_0.1</v>
+        <f t="shared" si="3"/>
+        <v>yolov8n_100e_0p_32b_SGD_512x512_0.07</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="1">
+        <v>100</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>16</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>yolov8n_100e_0p_16b_auto_512x512_0.07</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1">
+        <v>100</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>16</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>yolov8n_100e_0p_16b_Adam_512x512_0.07</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>yolov8n_100e_0p_16b_SGD_512x512_0.07</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>32</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" ref="I29:I40" si="4">_xlfn.CONCAT(C29, "_", D29, "e_",E29, "p_",F29, "b_",G29, "_",A29,"_",B29)</f>
+        <v>yolov8n_100e_0p_32b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1">
+        <v>100</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>32</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_100e_0p_32b_Adam_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1">
+        <v>100</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>32</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_100e_0p_32b_SGD_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1">
+        <v>100</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_100e_0p_16b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>16</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_100e_0p_16b_Adam_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1">
+        <v>100</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_100e_0p_16b_SGD_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1">
         <v>300</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E35" s="1">
         <v>50</v>
       </c>
-      <c r="F25" s="1">
-        <v>32</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F35" s="1">
+        <v>32</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_300e_50p_32b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1">
+        <v>300</v>
+      </c>
+      <c r="E36" s="1">
+        <v>50</v>
+      </c>
+      <c r="F36" s="1">
+        <v>32</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_300e_50p_32b_Adam_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1">
+        <v>300</v>
+      </c>
+      <c r="E37" s="1">
+        <v>50</v>
+      </c>
+      <c r="F37" s="1">
+        <v>32</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>yolov8n_300e_50p_32b_SGD_640x640_0.1</v>
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_300e_50p_32b_SGD_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="1">
+        <v>300</v>
+      </c>
+      <c r="E38" s="1">
+        <v>50</v>
+      </c>
+      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_300e_50p_16b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1">
+        <v>300</v>
+      </c>
+      <c r="E39" s="1">
+        <v>50</v>
+      </c>
+      <c r="F39" s="1">
+        <v>16</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_300e_50p_16b_Adam_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1">
+        <v>300</v>
+      </c>
+      <c r="E40" s="1">
+        <v>50</v>
+      </c>
+      <c r="F40" s="1">
+        <v>16</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>yolov8n_300e_50p_16b_SGD_320x320_0.12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Training"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{6A84E42F-A15A-48E5-9772-2C93CECE7943}">
+      <formula1>"Done, Training"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more trained models
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo ThinkBook\Documents\Thesis\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349B7196-E31A-47B7-888D-10B626D21902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4A8A30-77B4-45E7-8A09-F5CF58662C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="25">
   <si>
     <t>Epochs</t>
   </si>
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -837,6 +837,9 @@
       <c r="G11" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>yolov8n_300e_50p_32b_auto_640x640_0.2</v>
@@ -1003,7 +1006,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" ref="I18:I20" si="2">_xlfn.CONCAT(C18, "_", D18, "e_",E18, "p_",F18, "b_",G18, "_",A18,"_",B18)</f>
+        <f t="shared" ref="I18:I23" si="2">_xlfn.CONCAT(C18, "_", D18, "e_",E18, "p_",F18, "b_",G18, "_",A18,"_",B18)</f>
         <v>yolov8n_100e_0p_16b_auto_640x640_0.06</v>
       </c>
     </row>
@@ -1061,177 +1064,207 @@
         <v>yolov8n_100e_0p_16b_SGD_640x640_0.06</v>
       </c>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1">
+        <v>300</v>
+      </c>
+      <c r="E21" s="1">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1">
+        <v>32</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>yolov8n_300e_50p_32b_auto_640x640_0.06</v>
+      </c>
+    </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F22" s="1">
         <v>32</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" ref="I22:I27" si="3">_xlfn.CONCAT(C22, "_", D22, "e_",E22, "p_",F22, "b_",G22, "_",A22,"_",B22)</f>
-        <v>yolov8n_100e_0p_32b_auto_512x512_0.07</v>
+        <f t="shared" si="2"/>
+        <v>yolov8n_300e_50p_32b_Adam_640x640_0.06</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F23" s="1">
         <v>32</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>yolov8n_100e_0p_32b_Adam_512x512_0.07</v>
+        <f t="shared" si="2"/>
+        <v>yolov8n_300e_50p_32b_SGD_640x640_0.06</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E24" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F24" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>yolov8n_100e_0p_32b_SGD_512x512_0.07</v>
+        <f t="shared" ref="I24:I26" si="3">_xlfn.CONCAT(C24, "_", D24, "e_",E24, "p_",F24, "b_",G24, "_",A24,"_",B24)</f>
+        <v>yolov8n_300e_50p_16b_auto_640x640_0.06</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F25" s="1">
         <v>16</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>yolov8n_100e_0p_16b_auto_512x512_0.07</v>
+        <v>yolov8n_300e_50p_16b_Adam_640x640_0.06</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F26" s="1">
         <v>16</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>yolov8n_100e_0p_16b_Adam_512x512_0.07</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+        <v>yolov8n_300e_50p_16b_SGD_640x640_0.06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B28" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1">
-        <v>100</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <v>16</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>yolov8n_100e_0p_16b_SGD_512x512_0.07</v>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>100</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f t="shared" ref="I28:I33" si="4">_xlfn.CONCAT(C28, "_", D28, "e_",E28, "p_",F28, "b_",G28, "_",A28,"_",B28)</f>
+        <v>yolov8n_100e_0p_32b_auto_512x512_0.07</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -1246,22 +1279,19 @@
         <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I29" s="1" t="str">
-        <f t="shared" ref="I29:I40" si="4">_xlfn.CONCAT(C29, "_", D29, "e_",E29, "p_",F29, "b_",G29, "_",A29,"_",B29)</f>
-        <v>yolov8n_100e_0p_32b_auto_320x320_0.12</v>
+        <f t="shared" si="4"/>
+        <v>yolov8n_100e_0p_32b_Adam_512x512_0.07</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1276,19 +1306,19 @@
         <v>32</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>yolov8n_100e_0p_32b_Adam_320x320_0.12</v>
+        <v>yolov8n_100e_0p_32b_SGD_512x512_0.07</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -1300,22 +1330,22 @@
         <v>0</v>
       </c>
       <c r="F31" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>yolov8n_100e_0p_32b_SGD_320x320_0.12</v>
+        <v>yolov8n_100e_0p_16b_auto_512x512_0.07</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -1330,19 +1360,19 @@
         <v>16</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>yolov8n_100e_0p_16b_auto_320x320_0.12</v>
+        <v>yolov8n_100e_0p_16b_Adam_512x512_0.07</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1357,46 +1387,49 @@
         <v>16</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>yolov8n_100e_0p_16b_Adam_320x320_0.12</v>
+        <v>yolov8n_100e_0p_16b_SGD_512x512_0.07</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F34" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>yolov8n_100e_0p_16b_SGD_320x320_0.12</v>
+        <f t="shared" ref="I34:I39" si="5">_xlfn.CONCAT(C34, "_", D34, "e_",E34, "p_",F34, "b_",G34, "_",A34,"_",B34)</f>
+        <v>yolov8n_300e_50p_32b_auto_512x512_0.07</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>6</v>
@@ -1411,22 +1444,19 @@
         <v>32</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>yolov8n_300e_50p_32b_auto_320x320_0.12</v>
+        <f t="shared" si="5"/>
+        <v>yolov8n_300e_50p_32b_Adam_512x512_0.07</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -1441,19 +1471,19 @@
         <v>32</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I36" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>yolov8n_300e_50p_32b_Adam_320x320_0.12</v>
+        <f t="shared" si="5"/>
+        <v>yolov8n_300e_50p_32b_SGD_512x512_0.07</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
@@ -1465,22 +1495,22 @@
         <v>50</v>
       </c>
       <c r="F37" s="1">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>yolov8n_300e_50p_32b_SGD_320x320_0.12</v>
+        <f t="shared" si="5"/>
+        <v>yolov8n_300e_50p_16b_auto_512x512_0.07</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" s="1">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>6</v>
@@ -1495,64 +1525,367 @@
         <v>16</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>yolov8n_300e_50p_16b_auto_320x320_0.12</v>
+        <f t="shared" si="5"/>
+        <v>yolov8n_300e_50p_16b_Adam_512x512_0.07</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1">
+        <v>300</v>
+      </c>
+      <c r="E39" s="1">
+        <v>50</v>
+      </c>
+      <c r="F39" s="1">
+        <v>16</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>yolov8n_300e_50p_16b_SGD_512x512_0.07</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B41" s="1">
         <v>0.12</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="1">
-        <v>300</v>
-      </c>
-      <c r="E39" s="1">
-        <v>50</v>
-      </c>
-      <c r="F39" s="1">
-        <v>16</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="1">
+        <v>100</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>32</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f t="shared" ref="I41:I52" si="6">_xlfn.CONCAT(C41, "_", D41, "e_",E41, "p_",F41, "b_",G41, "_",A41,"_",B41)</f>
+        <v>yolov8n_100e_0p_32b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1">
+        <v>100</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>32</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="I42" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_100e_0p_32b_Adam_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1">
+        <v>100</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>32</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_100e_0p_32b_SGD_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="1">
+        <v>100</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>16</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I44" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_100e_0p_16b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1">
+        <v>100</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>16</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_100e_0p_16b_Adam_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="1">
+        <v>100</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>16</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_100e_0p_16b_SGD_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1">
+        <v>300</v>
+      </c>
+      <c r="E47" s="1">
+        <v>50</v>
+      </c>
+      <c r="F47" s="1">
+        <v>32</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_300e_50p_32b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="1">
+        <v>300</v>
+      </c>
+      <c r="E48" s="1">
+        <v>50</v>
+      </c>
+      <c r="F48" s="1">
+        <v>32</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_300e_50p_32b_Adam_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="1">
+        <v>300</v>
+      </c>
+      <c r="E49" s="1">
+        <v>50</v>
+      </c>
+      <c r="F49" s="1">
+        <v>32</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_300e_50p_32b_SGD_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1">
+        <v>300</v>
+      </c>
+      <c r="E50" s="1">
+        <v>50</v>
+      </c>
+      <c r="F50" s="1">
+        <v>16</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>yolov8n_300e_50p_16b_auto_320x320_0.12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="1">
+        <v>300</v>
+      </c>
+      <c r="E51" s="1">
+        <v>50</v>
+      </c>
+      <c r="F51" s="1">
+        <v>16</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>yolov8n_300e_50p_16b_Adam_320x320_0.12</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B52" s="1">
         <v>0.12</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="1">
-        <v>300</v>
-      </c>
-      <c r="E40" s="1">
-        <v>50</v>
-      </c>
-      <c r="F40" s="1">
-        <v>16</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="1">
+        <v>300</v>
+      </c>
+      <c r="E52" s="1">
+        <v>50</v>
+      </c>
+      <c r="F52" s="1">
+        <v>16</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="1" t="str">
-        <f t="shared" si="4"/>
+      <c r="I52" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>yolov8n_300e_50p_16b_SGD_320x320_0.12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added last 640_20 models
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Japh\Documents\Thesis2\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B6F588-01B5-423F-AAAB-BE13ED9D3354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC65DDCF-2017-4532-94E7-6AFB15F80940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="82">
   <si>
     <t>Epochs</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>3.5 hours + 0.678 hours</t>
+  </si>
+  <si>
+    <t>3.28 hours + 2.419 hours</t>
+  </si>
+  <si>
+    <t>3.3 hours + 2.340 hours</t>
   </si>
 </sst>
 </file>
@@ -644,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
-      <selection activeCell="O63" sqref="O63"/>
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2391,7 @@
         <v>11</v>
       </c>
       <c r="I56" s="1" t="str">
-        <f t="shared" ref="I56:I61" si="7">_xlfn.CONCAT(C56, "_", D56, "e_",E56, "p_",F56, "b_",G56, "_",A56,"_",B56)</f>
+        <f t="shared" ref="I56:I63" si="7">_xlfn.CONCAT(C56, "_", D56, "e_",E56, "p_",F56, "b_",G56, "_",A56,"_",B56)</f>
         <v>yolov8n_100e_0p_16b_AdamW_512_20</v>
       </c>
       <c r="J56" s="1" t="s">
@@ -2644,6 +2650,102 @@
         <v>0.73899999999999999</v>
       </c>
       <c r="O61" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>640</v>
+      </c>
+      <c r="B62" s="1">
+        <v>20</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="1">
+        <v>300</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>64</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I62" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>yolov8n_300e_0p_64b_SGD_640_20</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K62" s="1">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="L62" s="1">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="M62" s="1">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="N62" s="1">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>640</v>
+      </c>
+      <c r="B63" s="1">
+        <v>20</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="1">
+        <v>300</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>64</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>yolov8n_300e_0p_64b_AdamW_640_20</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K63" s="1">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="L63" s="1">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="M63" s="1">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="N63" s="1">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="O63" s="1" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>